<commit_message>
Note do an 23-Sep-2021
</commit_message>
<xml_diff>
--- a/Task_Assignment/Task_Assignment.xlsx
+++ b/Task_Assignment/Task_Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aptech\Sem_2\eProject2_Notes\Task_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CC673A-5AA7-4164-BDF8-2591B7D1B3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A99044-E558-4EF9-8DCD-27703EB3F03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7D0C622-867F-4336-B628-C253AAB18715}"/>
   </bookViews>
@@ -155,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -179,6 +179,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662BBCA7-EA8B-4776-B2B2-9EAA19CBB5BE}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -568,6 +571,9 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F8" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Share task assignment  Google docs link
</commit_message>
<xml_diff>
--- a/Task_Assignment/Task_Assignment.xlsx
+++ b/Task_Assignment/Task_Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aptech\Sem_2\eProject2_Notes\Task_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A99044-E558-4EF9-8DCD-27703EB3F03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5940E6FC-0AB4-40BB-B677-62EE9148F548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7D0C622-867F-4336-B628-C253AAB18715}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Status</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Bookstore Management</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -530,10 +533,12 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="J3" s="6" t="s">

</xml_diff>